<commit_message>
Updated notebooks to python 3.10
</commit_message>
<xml_diff>
--- a/data/meteo/nl1.xlsx
+++ b/data/meteo/nl1.xlsx
@@ -1,30 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\sources\pcse\pcse_notebooks\data\meteo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\UserData\sources\pcse\pcse_notebooks\data\meteo\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478851F5-FB43-4DD2-B28B-55E28C49F5A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="19155" windowHeight="9525"/>
+    <workbookView xWindow="0" yWindow="165" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ObservedWeather" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Wit, Allard de</author>
   </authors>
   <commentList>
-    <comment ref="A8" authorId="0" shapeId="0">
+    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -48,7 +62,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0" shapeId="0">
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -72,7 +86,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="0" shapeId="0">
+    <comment ref="C8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -96,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D8" authorId="0" shapeId="0">
+    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -120,7 +134,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="0" shapeId="0">
+    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -144,7 +158,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="0" shapeId="0">
+    <comment ref="F8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -168,7 +182,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A11" authorId="0" shapeId="0">
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -192,7 +206,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="0" shapeId="0">
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -216,7 +230,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="0" shapeId="0">
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -240,7 +254,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D11" authorId="0" shapeId="0">
+    <comment ref="D11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -264,7 +278,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E11" authorId="0" shapeId="0">
+    <comment ref="E11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -288,7 +302,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F11" authorId="0" shapeId="0">
+    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -312,7 +326,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G11" authorId="0" shapeId="0">
+    <comment ref="G11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -336,7 +350,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H11" authorId="0" shapeId="0">
+    <comment ref="H11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -472,7 +486,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -723,6 +737,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -758,6 +789,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -933,11 +981,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1839"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1040" workbookViewId="0">
-      <selection activeCell="A1109" sqref="A1109:XFD1110"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>